<commit_message>
transposing the shit requirements in the test souce file
</commit_message>
<xml_diff>
--- a/test/test_file.xlsx
+++ b/test/test_file.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="april_2025" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="history" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="team" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="shifts" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="shifts_requirements" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="week_requirements" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="holidays" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
@@ -391,6 +391,12 @@
     <t xml:space="preserve">shift_name</t>
   </si>
   <si>
+    <t xml:space="preserve">starting_hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_staff</t>
+  </si>
+  <si>
     <t xml:space="preserve">default_shift</t>
   </si>
   <si>
@@ -404,12 +410,6 @@
   </si>
   <si>
     <t xml:space="preserve">late_night_shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">starting_hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_staff</t>
   </si>
   <si>
     <t xml:space="preserve">monday</t>
@@ -3303,7 +3303,7 @@
   </sheetPr>
   <dimension ref="A1:AK96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -12170,44 +12170,44 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="str">
-        <f aca="false">"latest_" &amp; shifts!B$1</f>
-        <v>latest_default_shift</v>
+        <f aca="false">"latest_" &amp; shifts_requirements!B$1</f>
+        <v>latest_starting_hour</v>
       </c>
       <c r="D1" s="4" t="str">
-        <f aca="false">"latest_" &amp; shifts!C$1</f>
-        <v>latest_late_morning_shift</v>
+        <f aca="false">"latest_" &amp; shifts_requirements!C$1</f>
+        <v>latest_min_staff</v>
       </c>
       <c r="E1" s="4" t="str">
-        <f aca="false">"latest_" &amp; shifts!D$1</f>
-        <v>latest_evening_shift</v>
+        <f aca="false">"latest_" &amp; shifts_requirements!D$1</f>
+        <v>latest_min_skill_4</v>
       </c>
       <c r="F1" s="4" t="str">
-        <f aca="false">"latest_" &amp; shifts!E$1</f>
-        <v>latest_early_night_shift</v>
+        <f aca="false">"latest_" &amp; shifts_requirements!E$1</f>
+        <v>latest_min_</v>
       </c>
       <c r="G1" s="4" t="str">
-        <f aca="false">"latest_" &amp; shifts!F$1</f>
-        <v>latest_late_night_shift</v>
+        <f aca="false">"latest_" &amp; shifts_requirements!F$1</f>
+        <v>latest_min_</v>
       </c>
       <c r="H1" s="4" t="str">
-        <f aca="false">"num_" &amp; shifts!B$1</f>
-        <v>num_default_shift</v>
+        <f aca="false">"num_" &amp; shifts_requirements!B$1</f>
+        <v>num_starting_hour</v>
       </c>
       <c r="I1" s="4" t="str">
-        <f aca="false">"num_" &amp; shifts!C$1</f>
-        <v>num_late_morning_shift</v>
+        <f aca="false">"num_" &amp; shifts_requirements!C$1</f>
+        <v>num_min_staff</v>
       </c>
       <c r="J1" s="4" t="str">
-        <f aca="false">"num_" &amp; shifts!D$1</f>
-        <v>num_evening_shift</v>
+        <f aca="false">"num_" &amp; shifts_requirements!D$1</f>
+        <v>num_min_skill_4</v>
       </c>
       <c r="K1" s="4" t="str">
-        <f aca="false">"num_" &amp; shifts!E$1</f>
-        <v>num_early_night_shift</v>
+        <f aca="false">"num_" &amp; shifts_requirements!E$1</f>
+        <v>num_min_</v>
       </c>
       <c r="L1" s="4" t="str">
-        <f aca="false">"num_" &amp; shifts!F$1</f>
-        <v>num_late_night_shift</v>
+        <f aca="false">"num_" &amp; shifts_requirements!F$1</f>
+        <v>num_min_</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12536,24 +12536,24 @@
         <v>100</v>
       </c>
       <c r="H1" s="127" t="str">
-        <f aca="false">shifts!B1</f>
-        <v>default_shift</v>
+        <f aca="false">shifts_requirements!B1</f>
+        <v>starting_hour</v>
       </c>
       <c r="I1" s="124" t="str">
-        <f aca="false">shifts!C1</f>
-        <v>late_morning_shift</v>
+        <f aca="false">shifts_requirements!C1</f>
+        <v>min_staff</v>
       </c>
       <c r="J1" s="124" t="str">
-        <f aca="false">shifts!D1</f>
-        <v>evening_shift</v>
+        <f aca="false">shifts_requirements!D1</f>
+        <v>min_skill_4</v>
       </c>
       <c r="K1" s="124" t="str">
-        <f aca="false">shifts!E1</f>
-        <v>early_night_shift</v>
+        <f aca="false">shifts_requirements!E1</f>
+        <v>min_</v>
       </c>
       <c r="L1" s="124" t="str">
-        <f aca="false">shifts!F1</f>
-        <v>late_night_shift</v>
+        <f aca="false">shifts_requirements!F1</f>
+        <v>min_</v>
       </c>
       <c r="M1" s="127" t="s">
         <v>101</v>
@@ -19970,8 +19970,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19984,43 +19984,58 @@
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="124" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="4" t="str">
+        <f aca="false">"min_" &amp; team!P$1</f>
+        <v>min_skill_4</v>
+      </c>
+      <c r="E1" s="4" t="str">
+        <f aca="false">"min_" &amp; team!R$1</f>
+        <v>min_</v>
+      </c>
+      <c r="F1" s="4" t="str">
+        <f aca="false">"min_" &amp; team!T$1</f>
+        <v>min_</v>
+      </c>
+      <c r="G1" s="4" t="str">
+        <f aca="false">"min_" &amp; team!V$1</f>
+        <v>min_</v>
+      </c>
+      <c r="H1" s="4" t="str">
+        <f aca="false">"min_" &amp; team!X$1</f>
+        <v>min_</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="124" t="s">
-        <v>120</v>
       </c>
       <c r="B2" s="124" t="n">
         <v>8</v>
       </c>
       <c r="C2" s="124" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2" s="124" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2" s="124" t="n">
-        <v>13</v>
-      </c>
-      <c r="F2" s="124" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="I2" s="138"/>
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
@@ -20029,129 +20044,126 @@
       <c r="N2" s="138"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="124" t="s">
-        <v>121</v>
+      <c r="A3" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="124" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="124" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="124" t="n">
+      <c r="D3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="124" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" s="124" t="n">
         <v>5</v>
-      </c>
-      <c r="E3" s="124" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="124" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="str">
-        <f aca="false">"min_" &amp; team!M$1</f>
-        <v>min_skill_1</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>2</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="G4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="str">
-        <f aca="false">"min_" &amp; team!N$1</f>
-        <v>min_skill_2</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>3</v>
+      <c r="A5" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="124" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5" s="124" t="n">
+        <v>2</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="str">
-        <f aca="false">"min_" &amp; team!O$1</f>
-        <v>min_skill_3</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>2</v>
+      <c r="A6" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="124" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" s="124" t="n">
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="G6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="str">
-        <f aca="false">"min_" &amp; team!P$1</f>
-        <v>min_skill_4</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="str">
-        <f aca="false">"min_" &amp; team!Q$1</f>
-        <v>min_skill_5</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -20194,24 +20206,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="str">
-        <f aca="false">shifts!B1</f>
-        <v>default_shift</v>
+        <f aca="false">shifts_requirements!B1</f>
+        <v>starting_hour</v>
       </c>
       <c r="C1" s="4" t="str">
-        <f aca="false">shifts!C1</f>
-        <v>late_morning_shift</v>
+        <f aca="false">shifts_requirements!C1</f>
+        <v>min_staff</v>
       </c>
       <c r="D1" s="4" t="str">
-        <f aca="false">shifts!D1</f>
-        <v>evening_shift</v>
+        <f aca="false">shifts_requirements!D1</f>
+        <v>min_skill_4</v>
       </c>
       <c r="E1" s="4" t="str">
-        <f aca="false">shifts!E1</f>
-        <v>early_night_shift</v>
+        <f aca="false">shifts_requirements!E1</f>
+        <v>min_</v>
       </c>
       <c r="F1" s="4" t="str">
-        <f aca="false">shifts!F1</f>
-        <v>late_night_shift</v>
+        <f aca="false">shifts_requirements!F1</f>
+        <v>min_</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>